<commit_message>
added a upgradable save and fixed the income
</commit_message>
<xml_diff>
--- a/tier_info/money calc.xlsx
+++ b/tier_info/money calc.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arek\Desktop\discord_rpv2\tier_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arek\Desktop\Python projects\discord_rpv2\tier_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3BE16FF-4199-48EB-8DBC-47DD1EA8C2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2FA40D-1B56-4ED5-9A38-6EE1D7735C3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="money calc" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Tier</t>
   </si>
@@ -1087,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,12 +1096,11 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" hidden="1" customWidth="1"/>
-    <col min="13" max="15" width="14.28515625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="18" width="13.85546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="19" width="13.85546875" customWidth="1"/>
     <col min="20" max="20" width="13.7109375" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="10.5703125" customWidth="1"/>
     <col min="23" max="23" width="31.42578125" bestFit="1" customWidth="1"/>
@@ -1112,9 +1110,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
-        <f>W22</f>
-        <v>The Commonwealth of Utweiland</v>
+      <c r="A1" t="s">
+        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>55</v>
@@ -1148,6 +1145,9 @@
       </c>
       <c r="T1" s="4" t="s">
         <v>62</v>
+      </c>
+      <c r="X1" s="2">
+        <v>749923</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -1171,28 +1171,28 @@
       </c>
       <c r="H2" s="2">
         <f>VLOOKUP(A1, W2:AB33, 2, TRUE)</f>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="I2" s="2">
         <f>VLOOKUP(A1, W2:AB33, 3, TRUE)</f>
-        <v>205844</v>
+        <v>28521</v>
       </c>
       <c r="J2" s="2">
         <f>H2</f>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="1">
         <f>VLOOKUP(A1,W2:AB33, 5,TRUE)/100</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M2">
         <f>(M$13-1/20/5+1)</f>
-        <v>1.0900000000000001</v>
+        <v>1.44</v>
       </c>
       <c r="N2" s="1">
         <f>IF(N13&gt;0.5, 1, N13)</f>
-        <v>0.27</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1245,49 +1245,49 @@
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3:H12" si="0">ROUND((B3*D3+C3*E3)*0.01*$H$2, -5)</f>
-        <v>36000000</v>
+        <v>10100000</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3:I12" si="1">ROUND($I$2*F3, -3)</f>
-        <v>124000</v>
+        <v>17000</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J12" si="2">$J$2</f>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2">
         <f>L$2*H3</f>
-        <v>18000000</v>
+        <v>2525000</v>
       </c>
       <c r="M3" s="2">
         <f>M$2*L3</f>
-        <v>19620000</v>
+        <v>3636000</v>
       </c>
       <c r="N3" s="2">
         <f>N$2*M3</f>
-        <v>5297400</v>
+        <v>3636000</v>
       </c>
       <c r="O3" s="3">
         <f>L$2*M$2*N$2</f>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2">
         <f t="shared" ref="Q3:Q12" si="3">ROUND(H3-I3, -5)</f>
-        <v>35900000</v>
+        <v>10100000</v>
       </c>
       <c r="R3" s="2">
         <f t="shared" ref="R3:R12" si="4">M3-I3</f>
-        <v>19496000</v>
+        <v>3619000</v>
       </c>
       <c r="S3" s="2">
         <f>N3-I3</f>
-        <v>5173400</v>
+        <v>3619000</v>
       </c>
       <c r="T3" s="2">
         <f>S3-J3</f>
-        <v>2509410</v>
+        <v>2869077</v>
       </c>
       <c r="W3" t="s">
         <v>17</v>
@@ -1333,49 +1333,49 @@
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>44800000</v>
+        <v>12600000</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="1"/>
-        <v>309000</v>
+        <v>43000</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2">
         <f t="shared" ref="L4:L12" si="6">L$2*H4</f>
-        <v>22400000</v>
+        <v>3150000</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ref="M4:M12" si="7">M$2*L4</f>
-        <v>24416000</v>
+        <v>4536000</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" ref="N4:N12" si="8">N$2*M4</f>
-        <v>6592320</v>
+        <v>4536000</v>
       </c>
       <c r="O4" s="3">
         <f t="shared" ref="O4:O12" si="9">L$2*M$2*N$2</f>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2">
         <f t="shared" si="3"/>
-        <v>44500000</v>
+        <v>12600000</v>
       </c>
       <c r="R4" s="2">
         <f t="shared" si="4"/>
-        <v>24107000</v>
+        <v>4493000</v>
       </c>
       <c r="S4" s="2">
         <f t="shared" ref="S4:S12" si="10">N4-I4</f>
-        <v>6283320</v>
+        <v>4493000</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" ref="T4:T12" si="11">S4-J4</f>
-        <v>3619330</v>
+        <v>3743077</v>
       </c>
       <c r="W4" t="s">
         <v>18</v>
@@ -1421,49 +1421,49 @@
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>70300000</v>
+        <v>19800000</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>515000</v>
+        <v>71000</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2">
         <f t="shared" si="6"/>
-        <v>35150000</v>
+        <v>4950000</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="7"/>
-        <v>38313500</v>
+        <v>7128000</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="8"/>
-        <v>10344645</v>
+        <v>7128000</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2">
         <f t="shared" si="3"/>
-        <v>69800000</v>
+        <v>19700000</v>
       </c>
       <c r="R5" s="2">
         <f t="shared" si="4"/>
-        <v>37798500</v>
+        <v>7057000</v>
       </c>
       <c r="S5" s="2">
         <f t="shared" si="10"/>
-        <v>9829645</v>
+        <v>7057000</v>
       </c>
       <c r="T5" s="2">
         <f t="shared" si="11"/>
-        <v>7165655</v>
+        <v>6307077</v>
       </c>
       <c r="W5" t="s">
         <v>19</v>
@@ -1509,49 +1509,49 @@
       </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
-        <v>99100000</v>
+        <v>27900000</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>618000</v>
+        <v>86000</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2">
         <f t="shared" si="6"/>
-        <v>49550000</v>
+        <v>6975000</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" si="7"/>
-        <v>54009500.000000007</v>
+        <v>10044000</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="8"/>
-        <v>14582565.000000004</v>
+        <v>10044000</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2">
         <f t="shared" si="3"/>
-        <v>98500000</v>
+        <v>27800000</v>
       </c>
       <c r="R6" s="2">
         <f t="shared" si="4"/>
-        <v>53391500.000000007</v>
+        <v>9958000</v>
       </c>
       <c r="S6" s="2">
         <f t="shared" si="10"/>
-        <v>13964565.000000004</v>
+        <v>9958000</v>
       </c>
       <c r="T6" s="2">
         <f t="shared" si="11"/>
-        <v>11300575.000000004</v>
+        <v>9208077</v>
       </c>
       <c r="W6" t="s">
         <v>20</v>
@@ -1597,49 +1597,49 @@
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>43300000</v>
+        <v>12200000</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="1"/>
-        <v>4117000</v>
+        <v>570000</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2">
         <f t="shared" si="6"/>
-        <v>21650000</v>
+        <v>3050000</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" si="7"/>
-        <v>23598500</v>
+        <v>4392000</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="8"/>
-        <v>6371595</v>
+        <v>4392000</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2">
         <f t="shared" si="3"/>
-        <v>39200000</v>
+        <v>11600000</v>
       </c>
       <c r="R7" s="2">
         <f t="shared" si="4"/>
-        <v>19481500</v>
+        <v>3822000</v>
       </c>
       <c r="S7" s="2">
         <f t="shared" si="10"/>
-        <v>2254595</v>
+        <v>3822000</v>
       </c>
       <c r="T7" s="2">
         <f t="shared" si="11"/>
-        <v>-409395</v>
+        <v>3072077</v>
       </c>
       <c r="W7" t="s">
         <v>21</v>
@@ -1685,49 +1685,49 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>59900000</v>
+        <v>16900000</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>5764000</v>
+        <v>799000</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2">
         <f t="shared" si="6"/>
-        <v>29950000</v>
+        <v>4225000</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" si="7"/>
-        <v>32645500.000000004</v>
+        <v>6084000</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="8"/>
-        <v>8814285.0000000019</v>
+        <v>6084000</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2">
         <f t="shared" si="3"/>
-        <v>54100000</v>
+        <v>16100000</v>
       </c>
       <c r="R8" s="2">
         <f t="shared" si="4"/>
-        <v>26881500.000000004</v>
+        <v>5285000</v>
       </c>
       <c r="S8" s="2">
         <f t="shared" si="10"/>
-        <v>3050285.0000000019</v>
+        <v>5285000</v>
       </c>
       <c r="T8" s="2">
         <f t="shared" si="11"/>
-        <v>386295.00000000186</v>
+        <v>4535077</v>
       </c>
       <c r="W8" t="s">
         <v>22</v>
@@ -1773,49 +1773,49 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>88600000</v>
+        <v>24900000</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>7205000</v>
+        <v>998000</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2">
         <f t="shared" si="6"/>
-        <v>44300000</v>
+        <v>6225000</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" si="7"/>
-        <v>48287000</v>
+        <v>8964000</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="8"/>
-        <v>13037490</v>
+        <v>8964000</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2">
         <f t="shared" si="3"/>
-        <v>81400000</v>
+        <v>23900000</v>
       </c>
       <c r="R9" s="2">
         <f t="shared" si="4"/>
-        <v>41082000</v>
+        <v>7966000</v>
       </c>
       <c r="S9" s="2">
         <f t="shared" si="10"/>
-        <v>5832490</v>
+        <v>7966000</v>
       </c>
       <c r="T9" s="2">
         <f t="shared" si="11"/>
-        <v>3168500</v>
+        <v>7216077</v>
       </c>
       <c r="W9" t="s">
         <v>23</v>
@@ -1861,49 +1861,49 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>131200000</v>
+        <v>36900000</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>12351000</v>
+        <v>1711000</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2">
         <f t="shared" si="6"/>
-        <v>65600000</v>
+        <v>9225000</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="7"/>
-        <v>71504000</v>
+        <v>13284000</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="8"/>
-        <v>19306080</v>
+        <v>13284000</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2">
         <f t="shared" si="3"/>
-        <v>118800000</v>
+        <v>35200000</v>
       </c>
       <c r="R10" s="2">
         <f t="shared" si="4"/>
-        <v>59153000</v>
+        <v>11573000</v>
       </c>
       <c r="S10" s="2">
         <f t="shared" si="10"/>
-        <v>6955080</v>
+        <v>11573000</v>
       </c>
       <c r="T10" s="2">
         <f t="shared" si="11"/>
-        <v>4291090</v>
+        <v>10823077</v>
       </c>
       <c r="W10" t="s">
         <v>24</v>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>20800000</v>
+        <v>5800000</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
@@ -1957,41 +1957,41 @@
       </c>
       <c r="J11" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2">
         <f t="shared" si="6"/>
-        <v>10400000</v>
+        <v>1450000</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" si="7"/>
-        <v>11336000</v>
+        <v>2088000</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="8"/>
-        <v>3060720</v>
+        <v>2088000</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2">
         <f t="shared" si="3"/>
-        <v>20800000</v>
+        <v>5800000</v>
       </c>
       <c r="R11" s="2">
         <f t="shared" si="4"/>
-        <v>11336000</v>
+        <v>2088000</v>
       </c>
       <c r="S11" s="2">
         <f t="shared" si="10"/>
-        <v>3060720</v>
+        <v>2088000</v>
       </c>
       <c r="T11" s="2">
         <f t="shared" si="11"/>
-        <v>396730</v>
+        <v>1338077</v>
       </c>
       <c r="W11" t="s">
         <v>25</v>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>175800000</v>
+        <v>49500000</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="1"/>
@@ -2045,41 +2045,41 @@
       </c>
       <c r="J12" s="2">
         <f t="shared" si="2"/>
-        <v>2663990</v>
+        <v>749923</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2">
         <f t="shared" si="6"/>
-        <v>87900000</v>
+        <v>12375000</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" si="7"/>
-        <v>95811000</v>
+        <v>17820000</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" si="8"/>
-        <v>25868970</v>
+        <v>17820000</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" si="9"/>
-        <v>0.14715000000000003</v>
+        <v>0.36</v>
       </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2">
         <f t="shared" si="3"/>
-        <v>175800000</v>
+        <v>49500000</v>
       </c>
       <c r="R12" s="2">
         <f t="shared" si="4"/>
-        <v>95811000</v>
+        <v>17820000</v>
       </c>
       <c r="S12" s="2">
         <f t="shared" si="10"/>
-        <v>25868970</v>
+        <v>17820000</v>
       </c>
       <c r="T12" s="2">
         <f t="shared" si="11"/>
-        <v>23204980</v>
+        <v>17070077</v>
       </c>
       <c r="W12" t="s">
         <v>26</v>
@@ -2107,11 +2107,11 @@
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="M13" s="1">
         <f>VLOOKUP(A1, W2:AB33, 6, TRUE)/100</f>
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="N13">
         <f>VLOOKUP(A1, W2:AC33, 7, TRUE)/100</f>
-        <v>0.27</v>
+        <v>0.6</v>
       </c>
       <c r="W13" t="s">
         <v>27</v>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="B14" t="str">
         <f>IF(S3&gt;S7, "Rural", "Industrial")</f>
-        <v>Rural</v>
+        <v>Industrial</v>
       </c>
       <c r="W14" t="s">
         <v>28</v>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B15" t="str">
         <f>IF(S4&gt;S8, "Rural", "Industrial")</f>
-        <v>Rural</v>
+        <v>Industrial</v>
       </c>
       <c r="W15" t="s">
         <v>29</v>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="B16" t="str">
         <f>IF(S5&gt;S9, "Rural", "Industrial")</f>
-        <v>Rural</v>
+        <v>Industrial</v>
       </c>
       <c r="W16" t="s">
         <v>30</v>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="B17" t="str">
         <f>IF(S6&gt;S10, "Rural", "Industrial")</f>
-        <v>Rural</v>
+        <v>Industrial</v>
       </c>
       <c r="W17" t="s">
         <v>31</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="B18" s="2">
         <f>MIN(S3:S10)</f>
-        <v>2254595</v>
+        <v>3619000</v>
       </c>
       <c r="W18" t="s">
         <v>32</v>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B19" s="2">
         <f>MAX(S3:S10)</f>
-        <v>13964565.000000004</v>
+        <v>11573000</v>
       </c>
       <c r="W19" t="s">
         <v>33</v>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="B20" s="2">
         <f>AVERAGE(S3:S10)</f>
-        <v>6667922.5</v>
+        <v>6721625</v>
       </c>
       <c r="W20" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
added army hard save
</commit_message>
<xml_diff>
--- a/tier_info/money calc.xlsx
+++ b/tier_info/money calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arek\Desktop\Python projects\discord_rpv2\tier_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2FA40D-1B56-4ED5-9A38-6EE1D7735C3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6874C9E9-09E0-49B0-9E2F-221B9FC774BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1086,9 +1086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>